<commit_message>
adding assets thesis doc, and ppt
</commit_message>
<xml_diff>
--- a/Measurement Raw Data/Run264_Sep18_13-32_Sector 0_Hole A.xlsx
+++ b/Measurement Raw Data/Run264_Sep18_13-32_Sector 0_Hole A.xlsx
@@ -1,16 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28702"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jason/Documents/projects/ODU/Thesis/Measurement Raw Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="12435" windowHeight="4935" activeTab="1"/>
+    <workbookView xWindow="5880" yWindow="1540" windowWidth="21120" windowHeight="14280"/>
   </bookViews>
   <sheets>
     <sheet name="Run Data" sheetId="1" r:id="rId1"/>
     <sheet name="Run Info" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -117,16 +130,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -194,12 +207,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -229,12 +242,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -440,14 +453,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D211"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="13.5703125" customWidth="1"/>
+    <col min="1" max="4" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,7 +476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -475,7 +490,7 @@
         <v>-16.329000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -489,7 +504,7 @@
         <v>-15.423999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -503,7 +518,7 @@
         <v>-15.24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -517,7 +532,7 @@
         <v>-15.927</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -531,7 +546,7 @@
         <v>-16.411000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -545,7 +560,7 @@
         <v>-15.84</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -559,7 +574,7 @@
         <v>-15.599</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -573,7 +588,7 @@
         <v>-15.311</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -587,7 +602,7 @@
         <v>-15.43</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -601,7 +616,7 @@
         <v>-16.675999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -615,7 +630,7 @@
         <v>-16.289000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -629,7 +644,7 @@
         <v>-12.298</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -643,7 +658,7 @@
         <v>-13.065</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -657,7 +672,7 @@
         <v>-13.476000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -671,7 +686,7 @@
         <v>-13.023</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -685,7 +700,7 @@
         <v>-12.715999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -699,7 +714,7 @@
         <v>-12.855</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -713,7 +728,7 @@
         <v>-13.294</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -727,7 +742,7 @@
         <v>-14.911</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -741,7 +756,7 @@
         <v>-14.731</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -755,7 +770,7 @@
         <v>-13.840999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -769,7 +784,7 @@
         <v>-13.212999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -783,7 +798,7 @@
         <v>-12.433</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -797,7 +812,7 @@
         <v>-11.627000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -811,7 +826,7 @@
         <v>-10.792999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -825,7 +840,7 @@
         <v>-10.256</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -839,7 +854,7 @@
         <v>-10.053000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -853,7 +868,7 @@
         <v>-11.273999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -867,7 +882,7 @@
         <v>-11.43</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -881,7 +896,7 @@
         <v>-9.1489999999999991</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -895,7 +910,7 @@
         <v>-5.734</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -909,7 +924,7 @@
         <v>-2.3919999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -923,7 +938,7 @@
         <v>2.589</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -937,7 +952,7 @@
         <v>7.4459999999999997</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -951,7 +966,7 @@
         <v>13.416</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -965,7 +980,7 @@
         <v>20.602</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -979,7 +994,7 @@
         <v>27.907</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -993,7 +1008,7 @@
         <v>35.113999999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1007,7 +1022,7 @@
         <v>44.423999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1021,7 +1036,7 @@
         <v>54.009</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1035,7 +1050,7 @@
         <v>59.905000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1049,7 +1064,7 @@
         <v>65.652000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1063,7 +1078,7 @@
         <v>71.89</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1077,7 +1092,7 @@
         <v>82.266999999999996</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1091,7 +1106,7 @@
         <v>92.381</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1105,7 +1120,7 @@
         <v>89.316999999999993</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1119,7 +1134,7 @@
         <v>90.525000000000006</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1133,7 +1148,7 @@
         <v>92.543999999999997</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1147,7 +1162,7 @@
         <v>94.581999999999994</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1161,7 +1176,7 @@
         <v>97.963999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1175,7 +1190,7 @@
         <v>101.108</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1189,7 +1204,7 @@
         <v>97.296999999999997</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1203,7 +1218,7 @@
         <v>91.366</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1217,7 +1232,7 @@
         <v>89.57</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1231,7 +1246,7 @@
         <v>89.852999999999994</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1245,7 +1260,7 @@
         <v>91.465999999999994</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1259,7 +1274,7 @@
         <v>93.933000000000007</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -1273,7 +1288,7 @@
         <v>93.712999999999994</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -1287,7 +1302,7 @@
         <v>88.465000000000003</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -1301,7 +1316,7 @@
         <v>87.611999999999995</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -1315,7 +1330,7 @@
         <v>92.852999999999994</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -1329,7 +1344,7 @@
         <v>102.34</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -1343,7 +1358,7 @@
         <v>118.92100000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -1357,7 +1372,7 @@
         <v>136.54</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -1371,7 +1386,7 @@
         <v>149.32900000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -1385,7 +1400,7 @@
         <v>160.435</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -1399,7 +1414,7 @@
         <v>173.416</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -1413,7 +1428,7 @@
         <v>183.089</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -1427,7 +1442,7 @@
         <v>191.17500000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -1441,7 +1456,7 @@
         <v>195.05699999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -1455,7 +1470,7 @@
         <v>188.821</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -1469,7 +1484,7 @@
         <v>188.619</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -1483,7 +1498,7 @@
         <v>204.773</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -1497,7 +1512,7 @@
         <v>212.75</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -1511,7 +1526,7 @@
         <v>219.434</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -1525,7 +1540,7 @@
         <v>227.02099999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -1539,7 +1554,7 @@
         <v>225.005</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -1553,7 +1568,7 @@
         <v>219.733</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -1567,7 +1582,7 @@
         <v>212.94200000000001</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -1581,7 +1596,7 @@
         <v>199.47300000000001</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -1595,7 +1610,7 @@
         <v>194.22900000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -1609,7 +1624,7 @@
         <v>198.69</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -1623,7 +1638,7 @@
         <v>194.05600000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -1637,7 +1652,7 @@
         <v>195.26900000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -1651,7 +1666,7 @@
         <v>197.35</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -1665,7 +1680,7 @@
         <v>197.56100000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -1679,7 +1694,7 @@
         <v>194.708</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -1693,7 +1708,7 @@
         <v>188.018</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -1707,7 +1722,7 @@
         <v>172.036</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -1721,7 +1736,7 @@
         <v>157.49100000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -1735,7 +1750,7 @@
         <v>151.60499999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -1749,7 +1764,7 @@
         <v>154.99700000000001</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -1763,7 +1778,7 @@
         <v>165.61600000000001</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -1777,7 +1792,7 @@
         <v>180.982</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -1791,7 +1806,7 @@
         <v>189.38300000000001</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -1805,7 +1820,7 @@
         <v>195.47800000000001</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -1819,7 +1834,7 @@
         <v>198.03100000000001</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -1833,7 +1848,7 @@
         <v>196.59700000000001</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -1847,7 +1862,7 @@
         <v>192.58799999999999</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -1861,7 +1876,7 @@
         <v>187.70099999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -1875,7 +1890,7 @@
         <v>180.00800000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -1889,7 +1904,7 @@
         <v>165.82499999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -1903,7 +1918,7 @@
         <v>164.44800000000001</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -1917,7 +1932,7 @@
         <v>170.078</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -1931,7 +1946,7 @@
         <v>166.083</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -1945,7 +1960,7 @@
         <v>162.34</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -1959,7 +1974,7 @@
         <v>159.184</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -1973,7 +1988,7 @@
         <v>156.32900000000001</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -1987,7 +2002,7 @@
         <v>152.524</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -2001,7 +2016,7 @@
         <v>149.02199999999999</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -2015,7 +2030,7 @@
         <v>149.45500000000001</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -2029,7 +2044,7 @@
         <v>152.18199999999999</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -2043,7 +2058,7 @@
         <v>156.92599999999999</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -2057,7 +2072,7 @@
         <v>160.75200000000001</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -2071,7 +2086,7 @@
         <v>162.80699999999999</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -2085,7 +2100,7 @@
         <v>162.97900000000001</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -2099,7 +2114,7 @@
         <v>162.65</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -2113,7 +2128,7 @@
         <v>160.95599999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -2127,7 +2142,7 @@
         <v>155.541</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -2141,7 +2156,7 @@
         <v>143.506</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -2155,7 +2170,7 @@
         <v>140.46700000000001</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -2169,7 +2184,7 @@
         <v>145.172</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -2183,7 +2198,7 @@
         <v>152.62299999999999</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -2197,7 +2212,7 @@
         <v>167.114</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -2211,7 +2226,7 @@
         <v>182.148</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -2225,7 +2240,7 @@
         <v>193.57499999999999</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -2239,7 +2254,7 @@
         <v>190.09899999999999</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -2253,7 +2268,7 @@
         <v>184.95400000000001</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -2267,7 +2282,7 @@
         <v>183.4</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -2281,7 +2296,7 @@
         <v>180.98599999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -2295,7 +2310,7 @@
         <v>171.69300000000001</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -2309,7 +2324,7 @@
         <v>155.11000000000001</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -2323,7 +2338,7 @@
         <v>141.762</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -2337,7 +2352,7 @@
         <v>134.91800000000001</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -2351,7 +2366,7 @@
         <v>130.56899999999999</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -2365,7 +2380,7 @@
         <v>125.136</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -2379,7 +2394,7 @@
         <v>119.01600000000001</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -2393,7 +2408,7 @@
         <v>111.351</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -2407,7 +2422,7 @@
         <v>101.843</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -2421,7 +2436,7 @@
         <v>88.242999999999995</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -2435,7 +2450,7 @@
         <v>69.966999999999999</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -2449,7 +2464,7 @@
         <v>65.488</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -2463,7 +2478,7 @@
         <v>68.962000000000003</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -2477,7 +2492,7 @@
         <v>67.853999999999999</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -2491,7 +2506,7 @@
         <v>64.269000000000005</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -2505,7 +2520,7 @@
         <v>60.814</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -2519,7 +2534,7 @@
         <v>56.241</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -2533,7 +2548,7 @@
         <v>49.466000000000001</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -2547,7 +2562,7 @@
         <v>37.884</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -2561,7 +2576,7 @@
         <v>22.861999999999998</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -2575,7 +2590,7 @@
         <v>13.946</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -2589,7 +2604,7 @@
         <v>6.01</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -2603,7 +2618,7 @@
         <v>1.4279999999999999</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -2617,7 +2632,7 @@
         <v>4.0940000000000003</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -2631,7 +2646,7 @@
         <v>7.43</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -2645,7 +2660,7 @@
         <v>8.3420000000000005</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -2659,7 +2674,7 @@
         <v>2.738</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -2673,7 +2688,7 @@
         <v>-4.4720000000000004</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -2687,7 +2702,7 @@
         <v>-9.4280000000000008</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -2701,7 +2716,7 @@
         <v>-16.074999999999999</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -2715,7 +2730,7 @@
         <v>-23.937999999999999</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -2729,7 +2744,7 @@
         <v>-32.198999999999998</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -2743,7 +2758,7 @@
         <v>-39.53</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -2757,7 +2772,7 @@
         <v>-39.280999999999999</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -2771,7 +2786,7 @@
         <v>-41.017000000000003</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -2785,7 +2800,7 @@
         <v>-42.648000000000003</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -2799,7 +2814,7 @@
         <v>-43.39</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -2813,7 +2828,7 @@
         <v>-43.481999999999999</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -2827,7 +2842,7 @@
         <v>-45.238999999999997</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -2841,7 +2856,7 @@
         <v>-48.256999999999998</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -2855,7 +2870,7 @@
         <v>-52.017000000000003</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -2869,7 +2884,7 @@
         <v>-55.423999999999999</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -2883,7 +2898,7 @@
         <v>-52.988</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -2897,7 +2912,7 @@
         <v>-49.718000000000004</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -2911,7 +2926,7 @@
         <v>-48.091999999999999</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -2925,7 +2940,7 @@
         <v>-47.686999999999998</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -2939,7 +2954,7 @@
         <v>-47.301000000000002</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -2953,7 +2968,7 @@
         <v>-48.488</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -2967,7 +2982,7 @@
         <v>-51.377000000000002</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -2981,7 +2996,7 @@
         <v>-54.134</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -2995,7 +3010,7 @@
         <v>-57.473999999999997</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -3009,7 +3024,7 @@
         <v>-60.912999999999997</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -3023,7 +3038,7 @@
         <v>-62.326999999999998</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -3037,7 +3052,7 @@
         <v>-63.069000000000003</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -3051,7 +3066,7 @@
         <v>-63.448</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -3065,7 +3080,7 @@
         <v>-63.023000000000003</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -3079,7 +3094,7 @@
         <v>-61.771999999999998</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -3093,7 +3108,7 @@
         <v>-60.534999999999997</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -3107,7 +3122,7 @@
         <v>-59.048000000000002</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -3121,7 +3136,7 @@
         <v>-56.021000000000001</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -3135,7 +3150,7 @@
         <v>-52.587000000000003</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -3149,7 +3164,7 @@
         <v>-50.938000000000002</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -3163,7 +3178,7 @@
         <v>-49.463999999999999</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -3177,7 +3192,7 @@
         <v>-45.612000000000002</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -3191,7 +3206,7 @@
         <v>-42.526000000000003</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -3205,7 +3220,7 @@
         <v>-40.567</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -3219,7 +3234,7 @@
         <v>-38.752000000000002</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -3233,7 +3248,7 @@
         <v>-36.000999999999998</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -3247,7 +3262,7 @@
         <v>-33.531999999999996</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -3261,7 +3276,7 @@
         <v>-29.882000000000001</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -3275,7 +3290,7 @@
         <v>-21.509</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -3289,7 +3304,7 @@
         <v>-21.31</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -3303,7 +3318,7 @@
         <v>-21.317</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -3317,7 +3332,7 @@
         <v>-21.292000000000002</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -3331,7 +3346,7 @@
         <v>-21.331</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -3345,7 +3360,7 @@
         <v>-21.277999999999999</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -3359,7 +3374,7 @@
         <v>-21.31</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -3373,7 +3388,7 @@
         <v>-21.277999999999999</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -3387,7 +3402,7 @@
         <v>-21.279</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -3411,14 +3426,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="13.5703125" customWidth="1"/>
+    <col min="1" max="2" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -3426,7 +3443,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -3434,7 +3451,7 @@
         <v>42996.564163000003</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -3442,7 +3459,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -3450,7 +3467,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -3458,15 +3475,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -3474,7 +3491,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -3482,7 +3499,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -3490,7 +3507,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -3498,7 +3515,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>

</xml_diff>